<commit_message>
Added a training session
</commit_message>
<xml_diff>
--- a/scan_history.xlsx
+++ b/scan_history.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="2120" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="980" yWindow="2500" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="s300" sheetId="1" r:id="rId1"/>
     <sheet name="s304" sheetId="2" r:id="rId2"/>
+    <sheet name="s305" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -83,6 +84,9 @@
   </si>
   <si>
     <t>Performance looks good</t>
+  </si>
+  <si>
+    <t>Added catch trial runs</t>
   </si>
 </sst>
 </file>
@@ -599,10 +603,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -662,6 +666,29 @@
         <v>20</v>
       </c>
     </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2">
+        <v>42201</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -670,4 +697,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>